<commit_message>
Correccion de nombre en documentos errones
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1358 - RNCFAC, Carlos Mendoza, Oscar Daniel_MO/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2015/12/P1358 - RNCFAC, Carlos Mendoza, Oscar Daniel_MO/Calidad/No_conformidades.xlsx
@@ -88,7 +88,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,6 +133,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -209,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,6 +246,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -322,7 +332,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -394,7 +404,9 @@
       <c r="D4" s="5" t="n">
         <v>42361</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="n">
+        <v>42361</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
@@ -418,7 +430,9 @@
       <c r="D5" s="5" t="n">
         <v>42361</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="n">
+        <v>42361</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
@@ -442,7 +456,9 @@
       <c r="D6" s="5" t="n">
         <v>42359</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="n">
+        <v>42359</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
@@ -466,7 +482,9 @@
       <c r="D7" s="5" t="n">
         <v>42359</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="n">
+        <v>42359</v>
+      </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
@@ -477,7 +495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>5</v>
       </c>
@@ -490,7 +508,9 @@
       <c r="D8" s="5" t="n">
         <v>42359</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="8" t="n">
+        <v>42359</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>